<commit_message>
export to csv too
</commit_message>
<xml_diff>
--- a/scraped_ports.xlsx
+++ b/scraped_ports.xlsx
@@ -16,748 +16,748 @@
     <t>Port/TCP Information</t>
   </si>
   <si>
-    <t>Port: 20/TCP</t>
-  </si>
-  <si>
-    <t>Port: 21/TCP</t>
-  </si>
-  <si>
-    <t>Port: 22/TCP</t>
-  </si>
-  <si>
-    <t>Port: 23/TCP</t>
-  </si>
-  <si>
-    <t>Port: 25/TCP</t>
-  </si>
-  <si>
-    <t>Port: 27/TCP</t>
-  </si>
-  <si>
-    <t>Port: 28/TCP</t>
-  </si>
-  <si>
-    <t>Port: 39/TCP</t>
-  </si>
-  <si>
-    <t>Port: 44/TCP</t>
-  </si>
-  <si>
-    <t>Port: 52/TCP</t>
-  </si>
-  <si>
-    <t>Port: 53/TCP</t>
-  </si>
-  <si>
-    <t>Port: 54/TCP</t>
-  </si>
-  <si>
-    <t>Port: 69/TCP</t>
-  </si>
-  <si>
-    <t>Port: 80/TCP</t>
-  </si>
-  <si>
-    <t>Port: 102/TCP</t>
-  </si>
-  <si>
-    <t>Port: 105/TCP</t>
-  </si>
-  <si>
-    <t>Port: 113/TCP</t>
-  </si>
-  <si>
-    <t>Port: 123/TCP</t>
-  </si>
-  <si>
-    <t>Port: 137/UDP</t>
-  </si>
-  <si>
-    <t>Port: 146/TCP</t>
-  </si>
-  <si>
-    <t>Port: 146/UDP</t>
-  </si>
-  <si>
-    <t>Port: 200/TCP</t>
-  </si>
-  <si>
-    <t>Port: 222/TCP</t>
-  </si>
-  <si>
-    <t>Port: 285/TCP</t>
-  </si>
-  <si>
-    <t>Port: 370/TCP</t>
-  </si>
-  <si>
-    <t>Port: 420/TCP</t>
-  </si>
-  <si>
-    <t>Port: 555/TCP</t>
-  </si>
-  <si>
-    <t>Port: 589/TCP</t>
-  </si>
-  <si>
-    <t>Port: 650/TCP</t>
-  </si>
-  <si>
-    <t>Port: 666/TCP</t>
-  </si>
-  <si>
-    <t>Port: 668/TCP</t>
-  </si>
-  <si>
-    <t>Port: 669/TCP</t>
-  </si>
-  <si>
-    <t>Port: 692/TCP</t>
-  </si>
-  <si>
-    <t>Port: 777/TCP</t>
-  </si>
-  <si>
-    <t>Port: 831/TCP</t>
-  </si>
-  <si>
-    <t>Port: 901/TCP</t>
-  </si>
-  <si>
-    <t>Port: 902/TCP</t>
-  </si>
-  <si>
-    <t>Port: 903/TCP</t>
-  </si>
-  <si>
-    <t>Port: 956/TCP</t>
-  </si>
-  <si>
-    <t>Port: 999/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1000/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1001/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1005/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1010/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1011/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1012/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1015/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1016/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1024/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1025/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1025/UDP</t>
-  </si>
-  <si>
-    <t>Port: 1026/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1027/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1028/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1028/UDP</t>
-  </si>
-  <si>
-    <t>Port: 1029/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1029/UDP</t>
-  </si>
-  <si>
-    <t>Port: 1030/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1031/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1032/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1033/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1034/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1035/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1036/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1037/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1042/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1042/UDP</t>
-  </si>
-  <si>
-    <t>Port: 1044/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1044/UDP</t>
-  </si>
-  <si>
-    <t>Port: 1049/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1080/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1166/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1167/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1207/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1208/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1349/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1369/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1441/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1560/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1561/UDP</t>
-  </si>
-  <si>
-    <t>Port: 1826/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1911/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1967/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1983/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1984/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1985/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1991/TCP</t>
-  </si>
-  <si>
-    <t>Port: 1999/TCP</t>
-  </si>
-  <si>
-    <t>Port: 2000/TCP</t>
-  </si>
-  <si>
-    <t>Port: 2001/TCP</t>
-  </si>
-  <si>
-    <t>Port: 2002/TCP</t>
-  </si>
-  <si>
-    <t>Port: 2004/TCP</t>
-  </si>
-  <si>
-    <t>Port: 2005/TCP</t>
-  </si>
-  <si>
-    <t>Port: 2023/TCP</t>
-  </si>
-  <si>
-    <t>Port: 2150/TCP</t>
-  </si>
-  <si>
-    <t>Port: 2311/TCP</t>
-  </si>
-  <si>
-    <t>Port: 2332/TCP</t>
-  </si>
-  <si>
-    <t>Port: 2345/TCP</t>
-  </si>
-  <si>
-    <t>Port: 2583/TCP</t>
-  </si>
-  <si>
-    <t>Port: 2800/TCP</t>
-  </si>
-  <si>
-    <t>Port: 2929/TCP</t>
-  </si>
-  <si>
-    <t>Port: 2983/TCP</t>
-  </si>
-  <si>
-    <t>Port: 3000/TCP</t>
-  </si>
-  <si>
-    <t>Port: 3024/TCP</t>
-  </si>
-  <si>
-    <t>Port: 3031/TCP</t>
-  </si>
-  <si>
-    <t>Port: 3131/TCP</t>
-  </si>
-  <si>
-    <t>Port: 3410/TCP</t>
-  </si>
-  <si>
-    <t>Port: 3456/TCP</t>
-  </si>
-  <si>
-    <t>Port: 4092/TCP</t>
-  </si>
-  <si>
-    <t>Port: 4201/TCP</t>
-  </si>
-  <si>
-    <t>Port: 4225/TCP</t>
-  </si>
-  <si>
-    <t>Port: 4444/TCP</t>
-  </si>
-  <si>
-    <t>Port: 4653/TCP</t>
-  </si>
-  <si>
-    <t>Port: 4700/TCP</t>
-  </si>
-  <si>
-    <t>Port: 5000/TCP</t>
-  </si>
-  <si>
-    <t>Port: 5005/TCP</t>
-  </si>
-  <si>
-    <t>Port: 5025/TCP</t>
-  </si>
-  <si>
-    <t>Port: 5050/TCP</t>
-  </si>
-  <si>
-    <t>Port: 5151/TCP</t>
-  </si>
-  <si>
-    <t>Port: 5221/TCP</t>
-  </si>
-  <si>
-    <t>Port: 5695/TCP</t>
-  </si>
-  <si>
-    <t>Port: 5696/TCP</t>
-  </si>
-  <si>
-    <t>Port: 5697/TCP</t>
-  </si>
-  <si>
-    <t>Port: 5742/TCP</t>
-  </si>
-  <si>
-    <t>Port: 5873/TCP</t>
-  </si>
-  <si>
-    <t>Port: 5933/TCP</t>
-  </si>
-  <si>
-    <t>Port: 6000/TCP</t>
-  </si>
-  <si>
-    <t>Port: 6526/TCP</t>
-  </si>
-  <si>
-    <t>Port: 6667/TCP</t>
-  </si>
-  <si>
-    <t>Port: 6711/TCP</t>
-  </si>
-  <si>
-    <t>Port: 6969/TCP</t>
-  </si>
-  <si>
-    <t>Port: 7000/TCP</t>
-  </si>
-  <si>
-    <t>Port: 7007/TCP</t>
-  </si>
-  <si>
-    <t>Port: 7119/TCP</t>
-  </si>
-  <si>
-    <t>Port: 7290/TCP</t>
-  </si>
-  <si>
-    <t>Port: 7291/TCP</t>
-  </si>
-  <si>
-    <t>Port: 7626/TCP</t>
-  </si>
-  <si>
-    <t>Port: 7718/TCP</t>
-  </si>
-  <si>
-    <t>Port: 7800/TCP</t>
-  </si>
-  <si>
-    <t>Port: 7850/TCP</t>
-  </si>
-  <si>
-    <t>Port: 7878/TCP</t>
-  </si>
-  <si>
-    <t>Port: 7879/TCP</t>
-  </si>
-  <si>
-    <t>Port: 8012/TCP</t>
-  </si>
-  <si>
-    <t>Port: 8012/UDP</t>
-  </si>
-  <si>
-    <t>Port: 8811/TCP</t>
-  </si>
-  <si>
-    <t>Port: 8812/TCP</t>
-  </si>
-  <si>
-    <t>Port: 9117/TCP</t>
-  </si>
-  <si>
-    <t>Port: 9400/TCP</t>
-  </si>
-  <si>
-    <t>Port: 9401/TCP</t>
-  </si>
-  <si>
-    <t>Port: 9561/TCP</t>
-  </si>
-  <si>
-    <t>Port: 9563/TCP</t>
-  </si>
-  <si>
-    <t>Port: 9877/TCP</t>
-  </si>
-  <si>
-    <t>Port: 9878/TCP</t>
-  </si>
-  <si>
-    <t>Port: 9879/TCP</t>
-  </si>
-  <si>
-    <t>Port: 10001/TCP</t>
-  </si>
-  <si>
-    <t>Port: 10012/TCP</t>
-  </si>
-  <si>
-    <t>Port: 10013/TCP</t>
-  </si>
-  <si>
-    <t>Port: 10100/TCP</t>
-  </si>
-  <si>
-    <t>Port: 11000/TCP</t>
-  </si>
-  <si>
-    <t>Port: 11011/TCP</t>
-  </si>
-  <si>
-    <t>Port: 11111/TCP</t>
-  </si>
-  <si>
-    <t>Port: 11831/TCP</t>
-  </si>
-  <si>
-    <t>Port: 12000/TCP</t>
-  </si>
-  <si>
-    <t>Port: 12223/TCP</t>
-  </si>
-  <si>
-    <t>Port: 12345/TCP</t>
-  </si>
-  <si>
-    <t>Port: 12346/TCP</t>
-  </si>
-  <si>
-    <t>Port: 12348/TCP</t>
-  </si>
-  <si>
-    <t>Port: 12349/TCP</t>
-  </si>
-  <si>
-    <t>Port: 12973/TCP</t>
-  </si>
-  <si>
-    <t>Port: 12975/TCP</t>
-  </si>
-  <si>
-    <t>Port: 13223/TCP</t>
-  </si>
-  <si>
-    <t>Port: 13371/TCP</t>
-  </si>
-  <si>
-    <t>Port: 13500/TCP</t>
-  </si>
-  <si>
-    <t>Port: 14194/TCP</t>
-  </si>
-  <si>
-    <t>Port: 15000/TCP</t>
-  </si>
-  <si>
-    <t>Port: 15382/TCP</t>
-  </si>
-  <si>
-    <t>Port: 16057/TCP</t>
-  </si>
-  <si>
-    <t>Port: 16484/TCP</t>
-  </si>
-  <si>
-    <t>Port: 17499/TCP</t>
-  </si>
-  <si>
-    <t>Port: 17500/TCP</t>
-  </si>
-  <si>
-    <t>Port: 17569/TCP</t>
-  </si>
-  <si>
-    <t>Port: 20000/TCP</t>
-  </si>
-  <si>
-    <t>Port: 20001/TCP</t>
-  </si>
-  <si>
-    <t>Port: 20005/TCP</t>
-  </si>
-  <si>
-    <t>Port: 20331/TCP</t>
-  </si>
-  <si>
-    <t>Port: 21579/TCP</t>
-  </si>
-  <si>
-    <t>Port: 21957/TCP</t>
-  </si>
-  <si>
-    <t>Port: 22222/TCP</t>
-  </si>
-  <si>
-    <t>Port: 23023/TCP</t>
-  </si>
-  <si>
-    <t>Port: 23032/TCP</t>
-  </si>
-  <si>
-    <t>Port: 23321/TCP</t>
-  </si>
-  <si>
-    <t>Port: 24000/TCP</t>
-  </si>
-  <si>
-    <t>Port: 24289/TCP</t>
-  </si>
-  <si>
-    <t>Port: 25685/TCP</t>
-  </si>
-  <si>
-    <t>Port: 25686/TCP</t>
-  </si>
-  <si>
-    <t>Port: 25982/TCP</t>
-  </si>
-  <si>
-    <t>Port: 27160/TCP</t>
-  </si>
-  <si>
-    <t>Port: 27374/TCP</t>
-  </si>
-  <si>
-    <t>Port: 27379/TCP</t>
-  </si>
-  <si>
-    <t>Port: 28431/TCP</t>
-  </si>
-  <si>
-    <t>Port: 29559/TCP</t>
-  </si>
-  <si>
-    <t>Port: 29999/TCP</t>
-  </si>
-  <si>
-    <t>Port: 30000/TCP</t>
-  </si>
-  <si>
-    <t>Port: 30100/TCP</t>
-  </si>
-  <si>
-    <t>Port: 30101/TCP</t>
-  </si>
-  <si>
-    <t>Port: 30102/TCP</t>
-  </si>
-  <si>
-    <t>Port: 30103/UDP</t>
-  </si>
-  <si>
-    <t>Port: 30103/TCP</t>
-  </si>
-  <si>
-    <t>Port: 30133/TCP</t>
-  </si>
-  <si>
-    <t>Port: 30331/TCP</t>
-  </si>
-  <si>
-    <t>Port: 31557/TCP</t>
-  </si>
-  <si>
-    <t>Port: 31785/TCP</t>
-  </si>
-  <si>
-    <t>Port: 31787/TCP</t>
-  </si>
-  <si>
-    <t>Port: 31788/TCP</t>
-  </si>
-  <si>
-    <t>Port: 31789/TCP</t>
-  </si>
-  <si>
-    <t>Port: 31789/UDP</t>
-  </si>
-  <si>
-    <t>Port: 31790/TCP</t>
-  </si>
-  <si>
-    <t>Port: 31791/UDP</t>
-  </si>
-  <si>
-    <t>Port: 31791/TCP</t>
-  </si>
-  <si>
-    <t>Port: 31792/TCP</t>
-  </si>
-  <si>
-    <t>Port: 33333/TCP</t>
-  </si>
-  <si>
-    <t>Port: 34312/TCP</t>
-  </si>
-  <si>
-    <t>Port: 34313/TCP</t>
-  </si>
-  <si>
-    <t>Port: 34343/TCP</t>
-  </si>
-  <si>
-    <t>Port: 35000/TCP</t>
-  </si>
-  <si>
-    <t>Port: 35600/TCP</t>
-  </si>
-  <si>
-    <t>Port: 36794/TCP</t>
-  </si>
-  <si>
-    <t>Port: 38741/TCP</t>
-  </si>
-  <si>
-    <t>Port: 38742/TCP</t>
-  </si>
-  <si>
-    <t>Port: 40308/TCP</t>
-  </si>
-  <si>
-    <t>Port: 40412/TCP</t>
-  </si>
-  <si>
-    <t>Port: 44444/TCP</t>
-  </si>
-  <si>
-    <t>Port: 45454/TCP</t>
-  </si>
-  <si>
-    <t>Port: 47891/TCP</t>
-  </si>
-  <si>
-    <t>Port: 48004/TCP</t>
-  </si>
-  <si>
-    <t>Port: 48006/TCP</t>
-  </si>
-  <si>
-    <t>Port: 48512/TCP</t>
-  </si>
-  <si>
-    <t>Port: 49000/TCP</t>
-  </si>
-  <si>
-    <t>Port: 49301/TCP</t>
-  </si>
-  <si>
-    <t>Port: 50000/TCP</t>
-  </si>
-  <si>
-    <t>Port: 50021/TCP</t>
-  </si>
-  <si>
-    <t>Port: 50551/TCP</t>
-  </si>
-  <si>
-    <t>Port: 50552/TCP</t>
-  </si>
-  <si>
-    <t>Port: 55665/TCP</t>
-  </si>
-  <si>
-    <t>Port: 55666/TCP</t>
-  </si>
-  <si>
-    <t>Port: 56565/TCP</t>
-  </si>
-  <si>
-    <t>Port: 60551/TCP</t>
-  </si>
-  <si>
-    <t>Port: 60552/TCP</t>
+    <t>20/TCP</t>
+  </si>
+  <si>
+    <t>21/TCP</t>
+  </si>
+  <si>
+    <t>22/TCP</t>
+  </si>
+  <si>
+    <t>23/TCP</t>
+  </si>
+  <si>
+    <t>25/TCP</t>
+  </si>
+  <si>
+    <t>27/TCP</t>
+  </si>
+  <si>
+    <t>28/TCP</t>
+  </si>
+  <si>
+    <t>39/TCP</t>
+  </si>
+  <si>
+    <t>44/TCP</t>
+  </si>
+  <si>
+    <t>52/TCP</t>
+  </si>
+  <si>
+    <t>53/TCP</t>
+  </si>
+  <si>
+    <t>54/TCP</t>
+  </si>
+  <si>
+    <t>69/TCP</t>
+  </si>
+  <si>
+    <t>80/TCP</t>
+  </si>
+  <si>
+    <t>102/TCP</t>
+  </si>
+  <si>
+    <t>105/TCP</t>
+  </si>
+  <si>
+    <t>113/TCP</t>
+  </si>
+  <si>
+    <t>123/TCP</t>
+  </si>
+  <si>
+    <t>137/UDP</t>
+  </si>
+  <si>
+    <t>146/TCP</t>
+  </si>
+  <si>
+    <t>146/UDP</t>
+  </si>
+  <si>
+    <t>200/TCP</t>
+  </si>
+  <si>
+    <t>222/TCP</t>
+  </si>
+  <si>
+    <t>285/TCP</t>
+  </si>
+  <si>
+    <t>370/TCP</t>
+  </si>
+  <si>
+    <t>420/TCP</t>
+  </si>
+  <si>
+    <t>555/TCP</t>
+  </si>
+  <si>
+    <t>589/TCP</t>
+  </si>
+  <si>
+    <t>650/TCP</t>
+  </si>
+  <si>
+    <t>666/TCP</t>
+  </si>
+  <si>
+    <t>668/TCP</t>
+  </si>
+  <si>
+    <t>669/TCP</t>
+  </si>
+  <si>
+    <t>692/TCP</t>
+  </si>
+  <si>
+    <t>777/TCP</t>
+  </si>
+  <si>
+    <t>831/TCP</t>
+  </si>
+  <si>
+    <t>901/TCP</t>
+  </si>
+  <si>
+    <t>902/TCP</t>
+  </si>
+  <si>
+    <t>903/TCP</t>
+  </si>
+  <si>
+    <t>956/TCP</t>
+  </si>
+  <si>
+    <t>999/TCP</t>
+  </si>
+  <si>
+    <t>1000/TCP</t>
+  </si>
+  <si>
+    <t>1001/TCP</t>
+  </si>
+  <si>
+    <t>1005/TCP</t>
+  </si>
+  <si>
+    <t>1010/TCP</t>
+  </si>
+  <si>
+    <t>1011/TCP</t>
+  </si>
+  <si>
+    <t>1012/TCP</t>
+  </si>
+  <si>
+    <t>1015/TCP</t>
+  </si>
+  <si>
+    <t>1016/TCP</t>
+  </si>
+  <si>
+    <t>1024/TCP</t>
+  </si>
+  <si>
+    <t>1025/TCP</t>
+  </si>
+  <si>
+    <t>1025/UDP</t>
+  </si>
+  <si>
+    <t>1026/TCP</t>
+  </si>
+  <si>
+    <t>1027/TCP</t>
+  </si>
+  <si>
+    <t>1028/TCP</t>
+  </si>
+  <si>
+    <t>1028/UDP</t>
+  </si>
+  <si>
+    <t>1029/TCP</t>
+  </si>
+  <si>
+    <t>1029/UDP</t>
+  </si>
+  <si>
+    <t>1030/TCP</t>
+  </si>
+  <si>
+    <t>1031/TCP</t>
+  </si>
+  <si>
+    <t>1032/TCP</t>
+  </si>
+  <si>
+    <t>1033/TCP</t>
+  </si>
+  <si>
+    <t>1034/TCP</t>
+  </si>
+  <si>
+    <t>1035/TCP</t>
+  </si>
+  <si>
+    <t>1036/TCP</t>
+  </si>
+  <si>
+    <t>1037/TCP</t>
+  </si>
+  <si>
+    <t>1042/TCP</t>
+  </si>
+  <si>
+    <t>1042/UDP</t>
+  </si>
+  <si>
+    <t>1044/TCP</t>
+  </si>
+  <si>
+    <t>1044/UDP</t>
+  </si>
+  <si>
+    <t>1049/TCP</t>
+  </si>
+  <si>
+    <t>1080/TCP</t>
+  </si>
+  <si>
+    <t>1166/TCP</t>
+  </si>
+  <si>
+    <t>1167/TCP</t>
+  </si>
+  <si>
+    <t>1207/TCP</t>
+  </si>
+  <si>
+    <t>1208/TCP</t>
+  </si>
+  <si>
+    <t>1349/TCP</t>
+  </si>
+  <si>
+    <t>1369/TCP</t>
+  </si>
+  <si>
+    <t>1441/TCP</t>
+  </si>
+  <si>
+    <t>1560/TCP</t>
+  </si>
+  <si>
+    <t>1561/UDP</t>
+  </si>
+  <si>
+    <t>1826/TCP</t>
+  </si>
+  <si>
+    <t>1911/TCP</t>
+  </si>
+  <si>
+    <t>1967/TCP</t>
+  </si>
+  <si>
+    <t>1983/TCP</t>
+  </si>
+  <si>
+    <t>1984/TCP</t>
+  </si>
+  <si>
+    <t>1985/TCP</t>
+  </si>
+  <si>
+    <t>1991/TCP</t>
+  </si>
+  <si>
+    <t>1999/TCP</t>
+  </si>
+  <si>
+    <t>2000/TCP</t>
+  </si>
+  <si>
+    <t>2001/TCP</t>
+  </si>
+  <si>
+    <t>2002/TCP</t>
+  </si>
+  <si>
+    <t>2004/TCP</t>
+  </si>
+  <si>
+    <t>2005/TCP</t>
+  </si>
+  <si>
+    <t>2023/TCP</t>
+  </si>
+  <si>
+    <t>2150/TCP</t>
+  </si>
+  <si>
+    <t>2311/TCP</t>
+  </si>
+  <si>
+    <t>2332/TCP</t>
+  </si>
+  <si>
+    <t>2345/TCP</t>
+  </si>
+  <si>
+    <t>2583/TCP</t>
+  </si>
+  <si>
+    <t>2800/TCP</t>
+  </si>
+  <si>
+    <t>2929/TCP</t>
+  </si>
+  <si>
+    <t>2983/TCP</t>
+  </si>
+  <si>
+    <t>3000/TCP</t>
+  </si>
+  <si>
+    <t>3024/TCP</t>
+  </si>
+  <si>
+    <t>3031/TCP</t>
+  </si>
+  <si>
+    <t>3131/TCP</t>
+  </si>
+  <si>
+    <t>3410/TCP</t>
+  </si>
+  <si>
+    <t>3456/TCP</t>
+  </si>
+  <si>
+    <t>4092/TCP</t>
+  </si>
+  <si>
+    <t>4201/TCP</t>
+  </si>
+  <si>
+    <t>4225/TCP</t>
+  </si>
+  <si>
+    <t>4444/TCP</t>
+  </si>
+  <si>
+    <t>4653/TCP</t>
+  </si>
+  <si>
+    <t>4700/TCP</t>
+  </si>
+  <si>
+    <t>5000/TCP</t>
+  </si>
+  <si>
+    <t>5005/TCP</t>
+  </si>
+  <si>
+    <t>5025/TCP</t>
+  </si>
+  <si>
+    <t>5050/TCP</t>
+  </si>
+  <si>
+    <t>5151/TCP</t>
+  </si>
+  <si>
+    <t>5221/TCP</t>
+  </si>
+  <si>
+    <t>5695/TCP</t>
+  </si>
+  <si>
+    <t>5696/TCP</t>
+  </si>
+  <si>
+    <t>5697/TCP</t>
+  </si>
+  <si>
+    <t>5742/TCP</t>
+  </si>
+  <si>
+    <t>5873/TCP</t>
+  </si>
+  <si>
+    <t>5933/TCP</t>
+  </si>
+  <si>
+    <t>6000/TCP</t>
+  </si>
+  <si>
+    <t>6526/TCP</t>
+  </si>
+  <si>
+    <t>6667/TCP</t>
+  </si>
+  <si>
+    <t>6711/TCP</t>
+  </si>
+  <si>
+    <t>6969/TCP</t>
+  </si>
+  <si>
+    <t>7000/TCP</t>
+  </si>
+  <si>
+    <t>7007/TCP</t>
+  </si>
+  <si>
+    <t>7119/TCP</t>
+  </si>
+  <si>
+    <t>7290/TCP</t>
+  </si>
+  <si>
+    <t>7291/TCP</t>
+  </si>
+  <si>
+    <t>7626/TCP</t>
+  </si>
+  <si>
+    <t>7718/TCP</t>
+  </si>
+  <si>
+    <t>7800/TCP</t>
+  </si>
+  <si>
+    <t>7850/TCP</t>
+  </si>
+  <si>
+    <t>7878/TCP</t>
+  </si>
+  <si>
+    <t>7879/TCP</t>
+  </si>
+  <si>
+    <t>8012/TCP</t>
+  </si>
+  <si>
+    <t>8012/UDP</t>
+  </si>
+  <si>
+    <t>8811/TCP</t>
+  </si>
+  <si>
+    <t>8812/TCP</t>
+  </si>
+  <si>
+    <t>9117/TCP</t>
+  </si>
+  <si>
+    <t>9400/TCP</t>
+  </si>
+  <si>
+    <t>9401/TCP</t>
+  </si>
+  <si>
+    <t>9561/TCP</t>
+  </si>
+  <si>
+    <t>9563/TCP</t>
+  </si>
+  <si>
+    <t>9877/TCP</t>
+  </si>
+  <si>
+    <t>9878/TCP</t>
+  </si>
+  <si>
+    <t>9879/TCP</t>
+  </si>
+  <si>
+    <t>10001/TCP</t>
+  </si>
+  <si>
+    <t>10012/TCP</t>
+  </si>
+  <si>
+    <t>10013/TCP</t>
+  </si>
+  <si>
+    <t>10100/TCP</t>
+  </si>
+  <si>
+    <t>11000/TCP</t>
+  </si>
+  <si>
+    <t>11011/TCP</t>
+  </si>
+  <si>
+    <t>11111/TCP</t>
+  </si>
+  <si>
+    <t>11831/TCP</t>
+  </si>
+  <si>
+    <t>12000/TCP</t>
+  </si>
+  <si>
+    <t>12223/TCP</t>
+  </si>
+  <si>
+    <t>12345/TCP</t>
+  </si>
+  <si>
+    <t>12346/TCP</t>
+  </si>
+  <si>
+    <t>12348/TCP</t>
+  </si>
+  <si>
+    <t>12349/TCP</t>
+  </si>
+  <si>
+    <t>12973/TCP</t>
+  </si>
+  <si>
+    <t>12975/TCP</t>
+  </si>
+  <si>
+    <t>13223/TCP</t>
+  </si>
+  <si>
+    <t>13371/TCP</t>
+  </si>
+  <si>
+    <t>13500/TCP</t>
+  </si>
+  <si>
+    <t>14194/TCP</t>
+  </si>
+  <si>
+    <t>15000/TCP</t>
+  </si>
+  <si>
+    <t>15382/TCP</t>
+  </si>
+  <si>
+    <t>16057/TCP</t>
+  </si>
+  <si>
+    <t>16484/TCP</t>
+  </si>
+  <si>
+    <t>17499/TCP</t>
+  </si>
+  <si>
+    <t>17500/TCP</t>
+  </si>
+  <si>
+    <t>17569/TCP</t>
+  </si>
+  <si>
+    <t>20000/TCP</t>
+  </si>
+  <si>
+    <t>20001/TCP</t>
+  </si>
+  <si>
+    <t>20005/TCP</t>
+  </si>
+  <si>
+    <t>20331/TCP</t>
+  </si>
+  <si>
+    <t>21579/TCP</t>
+  </si>
+  <si>
+    <t>21957/TCP</t>
+  </si>
+  <si>
+    <t>22222/TCP</t>
+  </si>
+  <si>
+    <t>23023/TCP</t>
+  </si>
+  <si>
+    <t>23032/TCP</t>
+  </si>
+  <si>
+    <t>23321/TCP</t>
+  </si>
+  <si>
+    <t>24000/TCP</t>
+  </si>
+  <si>
+    <t>24289/TCP</t>
+  </si>
+  <si>
+    <t>25685/TCP</t>
+  </si>
+  <si>
+    <t>25686/TCP</t>
+  </si>
+  <si>
+    <t>25982/TCP</t>
+  </si>
+  <si>
+    <t>27160/TCP</t>
+  </si>
+  <si>
+    <t>27374/TCP</t>
+  </si>
+  <si>
+    <t>27379/TCP</t>
+  </si>
+  <si>
+    <t>28431/TCP</t>
+  </si>
+  <si>
+    <t>29559/TCP</t>
+  </si>
+  <si>
+    <t>29999/TCP</t>
+  </si>
+  <si>
+    <t>30000/TCP</t>
+  </si>
+  <si>
+    <t>30100/TCP</t>
+  </si>
+  <si>
+    <t>30101/TCP</t>
+  </si>
+  <si>
+    <t>30102/TCP</t>
+  </si>
+  <si>
+    <t>30103/UDP</t>
+  </si>
+  <si>
+    <t>30103/TCP</t>
+  </si>
+  <si>
+    <t>30133/TCP</t>
+  </si>
+  <si>
+    <t>30331/TCP</t>
+  </si>
+  <si>
+    <t>31557/TCP</t>
+  </si>
+  <si>
+    <t>31785/TCP</t>
+  </si>
+  <si>
+    <t>31787/TCP</t>
+  </si>
+  <si>
+    <t>31788/TCP</t>
+  </si>
+  <si>
+    <t>31789/TCP</t>
+  </si>
+  <si>
+    <t>31789/UDP</t>
+  </si>
+  <si>
+    <t>31790/TCP</t>
+  </si>
+  <si>
+    <t>31791/UDP</t>
+  </si>
+  <si>
+    <t>31791/TCP</t>
+  </si>
+  <si>
+    <t>31792/TCP</t>
+  </si>
+  <si>
+    <t>33333/TCP</t>
+  </si>
+  <si>
+    <t>34312/TCP</t>
+  </si>
+  <si>
+    <t>34313/TCP</t>
+  </si>
+  <si>
+    <t>34343/TCP</t>
+  </si>
+  <si>
+    <t>35000/TCP</t>
+  </si>
+  <si>
+    <t>35600/TCP</t>
+  </si>
+  <si>
+    <t>36794/TCP</t>
+  </si>
+  <si>
+    <t>38741/TCP</t>
+  </si>
+  <si>
+    <t>38742/TCP</t>
+  </si>
+  <si>
+    <t>40308/TCP</t>
+  </si>
+  <si>
+    <t>40412/TCP</t>
+  </si>
+  <si>
+    <t>44444/TCP</t>
+  </si>
+  <si>
+    <t>45454/TCP</t>
+  </si>
+  <si>
+    <t>47891/TCP</t>
+  </si>
+  <si>
+    <t>48004/TCP</t>
+  </si>
+  <si>
+    <t>48006/TCP</t>
+  </si>
+  <si>
+    <t>48512/TCP</t>
+  </si>
+  <si>
+    <t>49000/TCP</t>
+  </si>
+  <si>
+    <t>49301/TCP</t>
+  </si>
+  <si>
+    <t>50000/TCP</t>
+  </si>
+  <si>
+    <t>50021/TCP</t>
+  </si>
+  <si>
+    <t>50551/TCP</t>
+  </si>
+  <si>
+    <t>50552/TCP</t>
+  </si>
+  <si>
+    <t>55665/TCP</t>
+  </si>
+  <si>
+    <t>55666/TCP</t>
+  </si>
+  <si>
+    <t>56565/TCP</t>
+  </si>
+  <si>
+    <t>60551/TCP</t>
+  </si>
+  <si>
+    <t>60552/TCP</t>
   </si>
 </sst>
 </file>

</xml_diff>